<commit_message>
feat(etl): mejoras en pipeline de jugadores y carga semanal
</commit_message>
<xml_diff>
--- a/data/ref/calendario_partidos.xlsx
+++ b/data/ref/calendario_partidos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml-starter\chivas-ml\data\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7526C28-BBD4-4FDB-989A-A65303741162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059F76AA-2BC0-496D-A6D1-861B88FFBAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{502CE701-F65B-4157-9620-66B001A5B5F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{502CE701-F65B-4157-9620-66B001A5B5F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Fecha</t>
   </si>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +542,9 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">

</xml_diff>

<commit_message>
feat(etl): Lectura de archivos excel 97 - 2003
</commit_message>
<xml_diff>
--- a/data/ref/calendario_partidos.xlsx
+++ b/data/ref/calendario_partidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059F76AA-2BC0-496D-A6D1-861B88FFBAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F18E09-0A5D-4F40-9E30-0E56A57AA1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{502CE701-F65B-4157-9620-66B001A5B5F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Fecha</t>
   </si>
@@ -78,6 +78,45 @@
   </si>
   <si>
     <t>Cruz Azul</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Club America</t>
+  </si>
+  <si>
+    <t>Tigres</t>
+  </si>
+  <si>
+    <t>Toluca</t>
+  </si>
+  <si>
+    <t>Necaxa</t>
+  </si>
+  <si>
+    <t>Puebla</t>
+  </si>
+  <si>
+    <t>Pumas</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Mazatlan</t>
+  </si>
+  <si>
+    <t>Queretaro</t>
+  </si>
+  <si>
+    <t>Atlas</t>
+  </si>
+  <si>
+    <t>Pachuca</t>
+  </si>
+  <si>
+    <t>Monterrey</t>
   </si>
 </sst>
 </file>
@@ -450,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1231DA-56F3-4D2D-AEBB-98EA9F5E76AA}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +592,9 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -560,6 +602,152 @@
       </c>
       <c r="B10" t="s">
         <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45907</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45913</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45917</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45920</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45923</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45926</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45935</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45941</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45948</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45955</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45963</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45969</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>